<commit_message>
Added ws with scientific names
</commit_message>
<xml_diff>
--- a/Docs/Fish Indicator Species for EEP.xlsx
+++ b/Docs/Fish Indicator Species for EEP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\EEP_Tool\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" tabRatio="261"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" tabRatio="261" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
   <si>
     <t>Level III Ecoregion</t>
   </si>
@@ -238,6 +243,42 @@
   </si>
   <si>
     <t>Cover</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Scientific</t>
+  </si>
+  <si>
+    <t>Nocomis_leptocephalus</t>
+  </si>
+  <si>
+    <t>Etheostoma_flabellare</t>
+  </si>
+  <si>
+    <t>Aphredoderus_sayanus</t>
+  </si>
+  <si>
+    <t>Noturus_insignis</t>
+  </si>
+  <si>
+    <t>Moxostoma_collapsum</t>
+  </si>
+  <si>
+    <t>Percina_nevisense</t>
+  </si>
+  <si>
+    <t>Lepomis_auritus</t>
+  </si>
+  <si>
+    <t>Notropis_altipinnis</t>
+  </si>
+  <si>
+    <t>Clinostomus_funduloides</t>
+  </si>
+  <si>
+    <t>Etheostoma_olmstedi</t>
   </si>
 </sst>
 </file>
@@ -325,6 +366,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -372,7 +416,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,7 +451,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,7 +662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1172,12 +1218,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Modified to NOT run jackknife or create curves
</commit_message>
<xml_diff>
--- a/Docs/Fish Indicator Species for EEP.xlsx
+++ b/Docs/Fish Indicator Species for EEP.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\EEP_Tool\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\EEP\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" tabRatio="261" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25065" windowHeight="9840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Piedmont" sheetId="3" r:id="rId3"/>
+    <sheet name="MACP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="102">
   <si>
     <t>Level III Ecoregion</t>
   </si>
@@ -279,13 +280,61 @@
   </si>
   <si>
     <t>Etheostoma_olmstedi</t>
+  </si>
+  <si>
+    <t>CommonName</t>
+  </si>
+  <si>
+    <t>Anguilla rostrata</t>
+  </si>
+  <si>
+    <t>Umbra pygmaea</t>
+  </si>
+  <si>
+    <t>Esox americanus</t>
+  </si>
+  <si>
+    <t>Notropis cummingsae;Notropis procne;Notropis chalybaeus;Notropis altipinnis</t>
+  </si>
+  <si>
+    <t>Erimyzon oblongus;Minytrema melanops</t>
+  </si>
+  <si>
+    <t>Noturus gyrinus</t>
+  </si>
+  <si>
+    <t>Acantharchus pomotis</t>
+  </si>
+  <si>
+    <t>Enneacanthus gloriosus</t>
+  </si>
+  <si>
+    <t>Etheostoma olmstedi</t>
+  </si>
+  <si>
+    <t>Notropis_chlorocephalus</t>
+  </si>
+  <si>
+    <t>Notropis_procne</t>
+  </si>
+  <si>
+    <t>Notropis_chiliticus</t>
+  </si>
+  <si>
+    <t>Notropis_alborus</t>
+  </si>
+  <si>
+    <t>Etheostoma_nigrum</t>
+  </si>
+  <si>
+    <t>AdditionalSpp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +354,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -333,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -356,6 +413,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,9 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1220,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,12 +1391,244 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>